<commit_message>
formatted sheet "output" to not give NullPointerException
</commit_message>
<xml_diff>
--- a/src/main/resources/U5646616_2022_2022.xlsx
+++ b/src/main/resources/U5646616_2022_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indre\IdeaProjects\taxFormFiller\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE9BAFB-0B7F-4123-B864-9457DC61F7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ED4BA7-71A8-4639-A99C-E5C2EDE290F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Header</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Ameerika</t>
+  </si>
+  <si>
+    <t>emta</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1422,7 @@
   <dimension ref="A1:P110"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1553,18 +1556,40 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4" s="13"/>
+      <c r="G4" s="7">
+        <f ca="1">I2-G2</f>
+        <v>-8.1999999999999886</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E5" s="13"/>
+      <c r="G5" s="7">
+        <f ca="1">-H2</f>
+        <v>-1</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E6" s="13"/>
+      <c r="F6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="7">
+        <f ca="1">SUM(G4:G5)</f>
+        <v>-9.1999999999999886</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E7" s="13"/>
+      <c r="G7" s="7">
+        <v>-8.1199999999999992</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E8" s="13"/>
+      <c r="G8" s="7">
+        <f ca="1">G6/G7</f>
+        <v>1.133004926108373</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E9" s="13"/>
@@ -1879,17 +1904,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A7F08F-33F9-48F0-AAAE-375F06483D9F}">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
@@ -1899,11 +1923,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="str">
+      <c r="A1" s="16" t="str">
         <f>TransactionsFormatted!B2</f>
         <v>US0042251084</v>
       </c>
-      <c r="B1" s="4" t="str">
+      <c r="B1" s="16" t="str">
         <f>TransactionsFormatted!C2</f>
         <v>ACADIA PHARMACEUTICALS INC</v>
       </c>
@@ -1944,268 +1968,8 @@
         <v>USD</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D35" s="13"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D36" s="13"/>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D38" s="13"/>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D42" s="13"/>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D44" s="13"/>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D45" s="13"/>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D46" s="13"/>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D47" s="13"/>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D48" s="13"/>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" s="13"/>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D50" s="13"/>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D51" s="13"/>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D52" s="13"/>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D53" s="13"/>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D54" s="13"/>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D55" s="13"/>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D56" s="13"/>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D57" s="13"/>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D58" s="13"/>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D59" s="13"/>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D60" s="13"/>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D61" s="13"/>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D62" s="13"/>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D63" s="13"/>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D64" s="13"/>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D65" s="13"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D66" s="13"/>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D67" s="13"/>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D68" s="13"/>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D69" s="13"/>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D70" s="13"/>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D71" s="13"/>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D72" s="13"/>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D73" s="13"/>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D75" s="13"/>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D76" s="13"/>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D78" s="13"/>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D80" s="13"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D81" s="13"/>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D82" s="13"/>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D83" s="13"/>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D84" s="13"/>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D85" s="13"/>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D86" s="13"/>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D87" s="13"/>
-    </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D88" s="13"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>